<commit_message>
Organização das pastas e continuação das funções
</commit_message>
<xml_diff>
--- a/Relatorio/Gantt Chart.xlsx
+++ b/Relatorio/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26c96ee5941d8100/USP/3_Semestre/MAC0209/EP1/MAC0209-EP1/Relatorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="806" documentId="8_{B5793807-C7F4-4CB5-A5DA-C0234AC23292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC09585-A106-44AC-B5A9-184BF6CBF77F}"/>
+  <xr:revisionPtr revIDLastSave="812" documentId="8_{B5793807-C7F4-4CB5-A5DA-C0234AC23292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4576E335-DD04-49DC-8EAA-61C34D3CF2FB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A4FCB0B-57D2-4907-8438-4CD6B01FDF4D}"/>
   </bookViews>
@@ -493,6 +493,27 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,30 +542,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10852F43-F80D-4B6B-B8E6-5625F4B7831F}">
   <dimension ref="A1:DE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:V10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,116 +998,116 @@
     </row>
     <row r="2" spans="1:109" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="39" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-      <c r="AQ2" s="39"/>
-      <c r="AR2" s="39"/>
-      <c r="AS2" s="39"/>
-      <c r="AT2" s="39"/>
-      <c r="AU2" s="39"/>
-      <c r="AV2" s="39"/>
-      <c r="AW2" s="39"/>
-      <c r="AX2" s="39"/>
-      <c r="AY2" s="39"/>
-      <c r="AZ2" s="39"/>
-      <c r="BA2" s="25" t="s">
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="27"/>
+      <c r="AR2" s="27"/>
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="25"/>
-      <c r="BE2" s="25"/>
-      <c r="BF2" s="25"/>
-      <c r="BG2" s="25"/>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="25"/>
-      <c r="BK2" s="25"/>
-      <c r="BL2" s="25"/>
-      <c r="BM2" s="25"/>
-      <c r="BN2" s="25"/>
-      <c r="BO2" s="25"/>
-      <c r="BP2" s="25"/>
-      <c r="BQ2" s="25"/>
-      <c r="BR2" s="25"/>
-      <c r="BS2" s="25"/>
-      <c r="BT2" s="25"/>
-      <c r="BU2" s="25"/>
-      <c r="BV2" s="25"/>
-      <c r="BW2" s="25"/>
-      <c r="BX2" s="25"/>
-      <c r="BY2" s="25"/>
-      <c r="BZ2" s="25"/>
-      <c r="CA2" s="25"/>
-      <c r="CB2" s="25"/>
-      <c r="CC2" s="25"/>
-      <c r="CD2" s="25"/>
-      <c r="CE2" s="26" t="s">
+      <c r="BB2" s="36"/>
+      <c r="BC2" s="36"/>
+      <c r="BD2" s="36"/>
+      <c r="BE2" s="36"/>
+      <c r="BF2" s="36"/>
+      <c r="BG2" s="36"/>
+      <c r="BH2" s="36"/>
+      <c r="BI2" s="36"/>
+      <c r="BJ2" s="36"/>
+      <c r="BK2" s="36"/>
+      <c r="BL2" s="36"/>
+      <c r="BM2" s="36"/>
+      <c r="BN2" s="36"/>
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="36"/>
+      <c r="BT2" s="36"/>
+      <c r="BU2" s="36"/>
+      <c r="BV2" s="36"/>
+      <c r="BW2" s="36"/>
+      <c r="BX2" s="36"/>
+      <c r="BY2" s="36"/>
+      <c r="BZ2" s="36"/>
+      <c r="CA2" s="36"/>
+      <c r="CB2" s="36"/>
+      <c r="CC2" s="36"/>
+      <c r="CD2" s="36"/>
+      <c r="CE2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="CF2" s="26"/>
-      <c r="CG2" s="26"/>
-      <c r="CH2" s="26"/>
-      <c r="CI2" s="26"/>
-      <c r="CJ2" s="26"/>
-      <c r="CK2" s="26"/>
-      <c r="CL2" s="26"/>
-      <c r="CM2" s="26"/>
-      <c r="CN2" s="26"/>
-      <c r="CO2" s="26"/>
-      <c r="CP2" s="26"/>
-      <c r="CQ2" s="26"/>
+      <c r="CF2" s="37"/>
+      <c r="CG2" s="37"/>
+      <c r="CH2" s="37"/>
+      <c r="CI2" s="37"/>
+      <c r="CJ2" s="37"/>
+      <c r="CK2" s="37"/>
+      <c r="CL2" s="37"/>
+      <c r="CM2" s="37"/>
+      <c r="CN2" s="37"/>
+      <c r="CO2" s="37"/>
+      <c r="CP2" s="37"/>
+      <c r="CQ2" s="37"/>
       <c r="CR2" s="21"/>
       <c r="CS2" s="21"/>
       <c r="CT2" s="21"/>
@@ -1125,11 +1125,11 @@
     </row>
     <row r="3" spans="1:109" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="5">
         <v>16</v>
       </c>
@@ -1426,33 +1426,32 @@
       <c r="E4" s="22">
         <v>44689</v>
       </c>
-      <c r="F4" s="46">
-        <f>AVERAGE(F5:F12)</f>
-        <v>0.4375</v>
+      <c r="F4" s="23">
+        <v>0</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="37"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="45"/>
+      <c r="AB4" s="45"/>
+      <c r="AC4" s="46"/>
       <c r="AD4" s="11"/>
       <c r="AE4" s="11"/>
       <c r="AF4" s="11"/>
@@ -1536,18 +1535,18 @@
       <c r="E5" s="22">
         <v>44675</v>
       </c>
-      <c r="F5" s="46">
-        <v>1</v>
+      <c r="F5" s="23">
+        <v>0</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
@@ -1645,25 +1644,25 @@
       <c r="E6" s="22">
         <v>44682</v>
       </c>
-      <c r="F6" s="46">
-        <v>1</v>
+      <c r="F6" s="23">
+        <v>0</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
@@ -1754,21 +1753,21 @@
       <c r="E7" s="22">
         <v>44678</v>
       </c>
-      <c r="F7" s="46">
-        <v>0.5</v>
+      <c r="F7" s="23">
+        <v>0</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
       <c r="U7" s="10"/>
@@ -1863,8 +1862,8 @@
       <c r="E8" s="22">
         <v>44682</v>
       </c>
-      <c r="F8" s="46">
-        <v>0.5</v>
+      <c r="F8" s="23">
+        <v>0</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1875,13 +1874,13 @@
       <c r="M8" s="12"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
       <c r="W8" s="11"/>
       <c r="X8" s="11"/>
       <c r="Y8" s="11"/>
@@ -1972,8 +1971,8 @@
       <c r="E9" s="22">
         <v>44682</v>
       </c>
-      <c r="F9" s="46">
-        <v>0.5</v>
+      <c r="F9" s="23">
+        <v>0</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1984,13 +1983,13 @@
       <c r="M9" s="12"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="11"/>
@@ -2081,7 +2080,7 @@
       <c r="E10" s="22">
         <v>44682</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="23">
         <v>0</v>
       </c>
       <c r="G10" s="10"/>
@@ -2093,13 +2092,13 @@
       <c r="M10" s="12"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
       <c r="Y10" s="11"/>
@@ -2190,7 +2189,7 @@
       <c r="E11" s="22">
         <v>44683</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="23">
         <v>0</v>
       </c>
       <c r="G11" s="10"/>
@@ -2206,10 +2205,10 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
@@ -2299,7 +2298,7 @@
       <c r="E12" s="22">
         <v>44689</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="23">
         <v>0</v>
       </c>
       <c r="G12" s="10"/>
@@ -2317,14 +2316,14 @@
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
       <c r="U12" s="10"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="32"/>
-      <c r="AC12" s="32"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
       <c r="AD12" s="11"/>
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
@@ -2408,7 +2407,7 @@
       <c r="E13" s="22">
         <v>44734</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="23">
         <f>AVERAGE(F14:F22)</f>
         <v>0</v>
       </c>
@@ -2435,51 +2434,51 @@
       <c r="AA13" s="11"/>
       <c r="AB13" s="10"/>
       <c r="AC13" s="10"/>
-      <c r="AD13" s="43"/>
-      <c r="AE13" s="44"/>
-      <c r="AF13" s="44"/>
-      <c r="AG13" s="44"/>
-      <c r="AH13" s="44"/>
-      <c r="AI13" s="44"/>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="44"/>
-      <c r="AL13" s="44"/>
-      <c r="AM13" s="44"/>
-      <c r="AN13" s="44"/>
-      <c r="AO13" s="44"/>
-      <c r="AP13" s="44"/>
-      <c r="AQ13" s="44"/>
-      <c r="AR13" s="44"/>
-      <c r="AS13" s="44"/>
-      <c r="AT13" s="44"/>
-      <c r="AU13" s="44"/>
-      <c r="AV13" s="44"/>
-      <c r="AW13" s="44"/>
-      <c r="AX13" s="44"/>
-      <c r="AY13" s="44"/>
-      <c r="AZ13" s="44"/>
-      <c r="BA13" s="44"/>
-      <c r="BB13" s="44"/>
-      <c r="BC13" s="44"/>
-      <c r="BD13" s="44"/>
-      <c r="BE13" s="44"/>
-      <c r="BF13" s="44"/>
-      <c r="BG13" s="44"/>
-      <c r="BH13" s="44"/>
-      <c r="BI13" s="44"/>
-      <c r="BJ13" s="44"/>
-      <c r="BK13" s="44"/>
-      <c r="BL13" s="44"/>
-      <c r="BM13" s="44"/>
-      <c r="BN13" s="44"/>
-      <c r="BO13" s="44"/>
-      <c r="BP13" s="44"/>
-      <c r="BQ13" s="44"/>
-      <c r="BR13" s="44"/>
-      <c r="BS13" s="44"/>
-      <c r="BT13" s="44"/>
-      <c r="BU13" s="44"/>
-      <c r="BV13" s="45"/>
+      <c r="AD13" s="31"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="32"/>
+      <c r="AG13" s="32"/>
+      <c r="AH13" s="32"/>
+      <c r="AI13" s="32"/>
+      <c r="AJ13" s="32"/>
+      <c r="AK13" s="32"/>
+      <c r="AL13" s="32"/>
+      <c r="AM13" s="32"/>
+      <c r="AN13" s="32"/>
+      <c r="AO13" s="32"/>
+      <c r="AP13" s="32"/>
+      <c r="AQ13" s="32"/>
+      <c r="AR13" s="32"/>
+      <c r="AS13" s="32"/>
+      <c r="AT13" s="32"/>
+      <c r="AU13" s="32"/>
+      <c r="AV13" s="32"/>
+      <c r="AW13" s="32"/>
+      <c r="AX13" s="32"/>
+      <c r="AY13" s="32"/>
+      <c r="AZ13" s="32"/>
+      <c r="BA13" s="32"/>
+      <c r="BB13" s="32"/>
+      <c r="BC13" s="32"/>
+      <c r="BD13" s="32"/>
+      <c r="BE13" s="32"/>
+      <c r="BF13" s="32"/>
+      <c r="BG13" s="32"/>
+      <c r="BH13" s="32"/>
+      <c r="BI13" s="32"/>
+      <c r="BJ13" s="32"/>
+      <c r="BK13" s="32"/>
+      <c r="BL13" s="32"/>
+      <c r="BM13" s="32"/>
+      <c r="BN13" s="32"/>
+      <c r="BO13" s="32"/>
+      <c r="BP13" s="32"/>
+      <c r="BQ13" s="32"/>
+      <c r="BR13" s="32"/>
+      <c r="BS13" s="32"/>
+      <c r="BT13" s="32"/>
+      <c r="BU13" s="32"/>
+      <c r="BV13" s="33"/>
       <c r="BW13" s="11"/>
       <c r="BX13" s="11"/>
       <c r="BY13" s="10"/>
@@ -2518,7 +2517,7 @@
       <c r="E14" s="22">
         <v>44703</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="23">
         <v>0</v>
       </c>
       <c r="G14" s="10"/>
@@ -2544,20 +2543,20 @@
       <c r="AA14" s="11"/>
       <c r="AB14" s="10"/>
       <c r="AC14" s="10"/>
-      <c r="AD14" s="40"/>
-      <c r="AE14" s="41"/>
-      <c r="AF14" s="41"/>
-      <c r="AG14" s="41"/>
-      <c r="AH14" s="41"/>
-      <c r="AI14" s="41"/>
-      <c r="AJ14" s="41"/>
-      <c r="AK14" s="41"/>
-      <c r="AL14" s="41"/>
-      <c r="AM14" s="41"/>
-      <c r="AN14" s="41"/>
-      <c r="AO14" s="41"/>
-      <c r="AP14" s="41"/>
-      <c r="AQ14" s="42"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AH14" s="29"/>
+      <c r="AI14" s="29"/>
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29"/>
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="29"/>
+      <c r="AN14" s="29"/>
+      <c r="AO14" s="29"/>
+      <c r="AP14" s="29"/>
+      <c r="AQ14" s="30"/>
       <c r="AR14" s="11"/>
       <c r="AS14" s="11"/>
       <c r="AT14" s="11"/>
@@ -2627,7 +2626,7 @@
       <c r="E15" s="22">
         <v>44703</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="23">
         <v>0</v>
       </c>
       <c r="G15" s="10"/>
@@ -2653,20 +2652,20 @@
       <c r="AA15" s="11"/>
       <c r="AB15" s="10"/>
       <c r="AC15" s="10"/>
-      <c r="AD15" s="40"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="41"/>
-      <c r="AG15" s="41"/>
-      <c r="AH15" s="41"/>
-      <c r="AI15" s="41"/>
-      <c r="AJ15" s="41"/>
-      <c r="AK15" s="41"/>
-      <c r="AL15" s="41"/>
-      <c r="AM15" s="41"/>
-      <c r="AN15" s="41"/>
-      <c r="AO15" s="41"/>
-      <c r="AP15" s="41"/>
-      <c r="AQ15" s="42"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="29"/>
+      <c r="AF15" s="29"/>
+      <c r="AG15" s="29"/>
+      <c r="AH15" s="29"/>
+      <c r="AI15" s="29"/>
+      <c r="AJ15" s="29"/>
+      <c r="AK15" s="29"/>
+      <c r="AL15" s="29"/>
+      <c r="AM15" s="29"/>
+      <c r="AN15" s="29"/>
+      <c r="AO15" s="29"/>
+      <c r="AP15" s="29"/>
+      <c r="AQ15" s="30"/>
       <c r="AR15" s="11"/>
       <c r="AS15" s="11"/>
       <c r="AT15" s="11"/>
@@ -2736,7 +2735,7 @@
       <c r="E16" s="22">
         <v>44715</v>
       </c>
-      <c r="F16" s="46">
+      <c r="F16" s="23">
         <v>0</v>
       </c>
       <c r="G16" s="10"/>
@@ -2776,18 +2775,18 @@
       <c r="AO16" s="11"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
-      <c r="AR16" s="40"/>
-      <c r="AS16" s="41"/>
-      <c r="AT16" s="41"/>
-      <c r="AU16" s="41"/>
-      <c r="AV16" s="41"/>
-      <c r="AW16" s="41"/>
-      <c r="AX16" s="41"/>
-      <c r="AY16" s="41"/>
-      <c r="AZ16" s="41"/>
-      <c r="BA16" s="41"/>
-      <c r="BB16" s="41"/>
-      <c r="BC16" s="42"/>
+      <c r="AR16" s="28"/>
+      <c r="AS16" s="29"/>
+      <c r="AT16" s="29"/>
+      <c r="AU16" s="29"/>
+      <c r="AV16" s="29"/>
+      <c r="AW16" s="29"/>
+      <c r="AX16" s="29"/>
+      <c r="AY16" s="29"/>
+      <c r="AZ16" s="29"/>
+      <c r="BA16" s="29"/>
+      <c r="BB16" s="29"/>
+      <c r="BC16" s="30"/>
       <c r="BD16" s="10"/>
       <c r="BE16" s="10"/>
       <c r="BF16" s="11"/>
@@ -2845,7 +2844,7 @@
       <c r="E17" s="22">
         <v>44715</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F17" s="23">
         <v>0</v>
       </c>
       <c r="G17" s="10"/>
@@ -2885,18 +2884,18 @@
       <c r="AO17" s="11"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
-      <c r="AR17" s="40"/>
-      <c r="AS17" s="41"/>
-      <c r="AT17" s="41"/>
-      <c r="AU17" s="41"/>
-      <c r="AV17" s="41"/>
-      <c r="AW17" s="41"/>
-      <c r="AX17" s="41"/>
-      <c r="AY17" s="41"/>
-      <c r="AZ17" s="41"/>
-      <c r="BA17" s="41"/>
-      <c r="BB17" s="41"/>
-      <c r="BC17" s="42"/>
+      <c r="AR17" s="28"/>
+      <c r="AS17" s="29"/>
+      <c r="AT17" s="29"/>
+      <c r="AU17" s="29"/>
+      <c r="AV17" s="29"/>
+      <c r="AW17" s="29"/>
+      <c r="AX17" s="29"/>
+      <c r="AY17" s="29"/>
+      <c r="AZ17" s="29"/>
+      <c r="BA17" s="29"/>
+      <c r="BB17" s="29"/>
+      <c r="BC17" s="30"/>
       <c r="BD17" s="10"/>
       <c r="BE17" s="10"/>
       <c r="BF17" s="11"/>
@@ -2954,7 +2953,7 @@
       <c r="E18" s="22">
         <v>44734</v>
       </c>
-      <c r="F18" s="46">
+      <c r="F18" s="23">
         <v>0</v>
       </c>
       <c r="G18" s="10"/>
@@ -3000,31 +2999,31 @@
       <c r="AU18" s="11"/>
       <c r="AV18" s="11"/>
       <c r="AW18" s="20"/>
-      <c r="AX18" s="40"/>
-      <c r="AY18" s="41"/>
-      <c r="AZ18" s="41"/>
-      <c r="BA18" s="41"/>
-      <c r="BB18" s="41"/>
-      <c r="BC18" s="41"/>
-      <c r="BD18" s="41"/>
-      <c r="BE18" s="41"/>
-      <c r="BF18" s="41"/>
-      <c r="BG18" s="41"/>
-      <c r="BH18" s="41"/>
-      <c r="BI18" s="41"/>
-      <c r="BJ18" s="41"/>
-      <c r="BK18" s="41"/>
-      <c r="BL18" s="41"/>
-      <c r="BM18" s="41"/>
-      <c r="BN18" s="41"/>
-      <c r="BO18" s="41"/>
-      <c r="BP18" s="41"/>
-      <c r="BQ18" s="41"/>
-      <c r="BR18" s="41"/>
-      <c r="BS18" s="41"/>
-      <c r="BT18" s="41"/>
-      <c r="BU18" s="41"/>
-      <c r="BV18" s="42"/>
+      <c r="AX18" s="28"/>
+      <c r="AY18" s="29"/>
+      <c r="AZ18" s="29"/>
+      <c r="BA18" s="29"/>
+      <c r="BB18" s="29"/>
+      <c r="BC18" s="29"/>
+      <c r="BD18" s="29"/>
+      <c r="BE18" s="29"/>
+      <c r="BF18" s="29"/>
+      <c r="BG18" s="29"/>
+      <c r="BH18" s="29"/>
+      <c r="BI18" s="29"/>
+      <c r="BJ18" s="29"/>
+      <c r="BK18" s="29"/>
+      <c r="BL18" s="29"/>
+      <c r="BM18" s="29"/>
+      <c r="BN18" s="29"/>
+      <c r="BO18" s="29"/>
+      <c r="BP18" s="29"/>
+      <c r="BQ18" s="29"/>
+      <c r="BR18" s="29"/>
+      <c r="BS18" s="29"/>
+      <c r="BT18" s="29"/>
+      <c r="BU18" s="29"/>
+      <c r="BV18" s="30"/>
       <c r="BW18" s="11"/>
       <c r="BX18" s="11"/>
       <c r="BY18" s="10"/>
@@ -3063,7 +3062,7 @@
       <c r="E19" s="22">
         <v>44724</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="23">
         <v>0</v>
       </c>
       <c r="G19" s="10"/>
@@ -3115,15 +3114,15 @@
       <c r="BA19" s="11"/>
       <c r="BB19" s="11"/>
       <c r="BC19" s="11"/>
-      <c r="BD19" s="40"/>
-      <c r="BE19" s="41"/>
-      <c r="BF19" s="41"/>
-      <c r="BG19" s="41"/>
-      <c r="BH19" s="41"/>
-      <c r="BI19" s="41"/>
-      <c r="BJ19" s="41"/>
-      <c r="BK19" s="41"/>
-      <c r="BL19" s="42"/>
+      <c r="BD19" s="28"/>
+      <c r="BE19" s="29"/>
+      <c r="BF19" s="29"/>
+      <c r="BG19" s="29"/>
+      <c r="BH19" s="29"/>
+      <c r="BI19" s="29"/>
+      <c r="BJ19" s="29"/>
+      <c r="BK19" s="29"/>
+      <c r="BL19" s="30"/>
       <c r="BM19" s="12"/>
       <c r="BN19" s="12"/>
       <c r="BO19" s="12"/>
@@ -3172,7 +3171,7 @@
       <c r="E20" s="22">
         <v>44724</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="23">
         <v>0</v>
       </c>
       <c r="G20" s="10"/>
@@ -3224,15 +3223,15 @@
       <c r="BA20" s="11"/>
       <c r="BB20" s="11"/>
       <c r="BC20" s="11"/>
-      <c r="BD20" s="40"/>
-      <c r="BE20" s="41"/>
-      <c r="BF20" s="41"/>
-      <c r="BG20" s="41"/>
-      <c r="BH20" s="41"/>
-      <c r="BI20" s="41"/>
-      <c r="BJ20" s="41"/>
-      <c r="BK20" s="41"/>
-      <c r="BL20" s="42"/>
+      <c r="BD20" s="28"/>
+      <c r="BE20" s="29"/>
+      <c r="BF20" s="29"/>
+      <c r="BG20" s="29"/>
+      <c r="BH20" s="29"/>
+      <c r="BI20" s="29"/>
+      <c r="BJ20" s="29"/>
+      <c r="BK20" s="29"/>
+      <c r="BL20" s="30"/>
       <c r="BM20" s="12"/>
       <c r="BN20" s="12"/>
       <c r="BO20" s="12"/>
@@ -3281,7 +3280,7 @@
       <c r="E21" s="22">
         <v>44729</v>
       </c>
-      <c r="F21" s="46">
+      <c r="F21" s="23">
         <v>0</v>
       </c>
       <c r="G21" s="10"/>
@@ -3338,15 +3337,15 @@
       <c r="BF21" s="11"/>
       <c r="BG21" s="11"/>
       <c r="BH21" s="11"/>
-      <c r="BI21" s="40"/>
-      <c r="BJ21" s="41"/>
-      <c r="BK21" s="41"/>
-      <c r="BL21" s="41"/>
-      <c r="BM21" s="41"/>
-      <c r="BN21" s="41"/>
-      <c r="BO21" s="41"/>
-      <c r="BP21" s="41"/>
-      <c r="BQ21" s="42"/>
+      <c r="BI21" s="28"/>
+      <c r="BJ21" s="29"/>
+      <c r="BK21" s="29"/>
+      <c r="BL21" s="29"/>
+      <c r="BM21" s="29"/>
+      <c r="BN21" s="29"/>
+      <c r="BO21" s="29"/>
+      <c r="BP21" s="29"/>
+      <c r="BQ21" s="30"/>
       <c r="BR21" s="10"/>
       <c r="BS21" s="10"/>
       <c r="BT21" s="11"/>
@@ -3390,7 +3389,7 @@
       <c r="E22" s="22">
         <v>44730</v>
       </c>
-      <c r="F22" s="46">
+      <c r="F22" s="23">
         <v>0</v>
       </c>
       <c r="G22" s="10"/>
@@ -3447,15 +3446,15 @@
       <c r="BF22" s="11"/>
       <c r="BG22" s="11"/>
       <c r="BH22" s="11"/>
-      <c r="BI22" s="40"/>
-      <c r="BJ22" s="41"/>
-      <c r="BK22" s="41"/>
-      <c r="BL22" s="41"/>
-      <c r="BM22" s="41"/>
-      <c r="BN22" s="41"/>
-      <c r="BO22" s="41"/>
-      <c r="BP22" s="41"/>
-      <c r="BQ22" s="42"/>
+      <c r="BI22" s="28"/>
+      <c r="BJ22" s="29"/>
+      <c r="BK22" s="29"/>
+      <c r="BL22" s="29"/>
+      <c r="BM22" s="29"/>
+      <c r="BN22" s="29"/>
+      <c r="BO22" s="29"/>
+      <c r="BP22" s="29"/>
+      <c r="BQ22" s="30"/>
       <c r="BR22" s="10"/>
       <c r="BS22" s="10"/>
       <c r="BT22" s="11"/>
@@ -3499,7 +3498,7 @@
       <c r="E23" s="22">
         <v>44729</v>
       </c>
-      <c r="F23" s="46">
+      <c r="F23" s="23">
         <f>F24</f>
         <v>0</v>
       </c>
@@ -3571,14 +3570,14 @@
       <c r="BT23" s="11"/>
       <c r="BU23" s="11"/>
       <c r="BV23" s="11"/>
-      <c r="BW23" s="23"/>
-      <c r="BX23" s="24"/>
-      <c r="BY23" s="24"/>
-      <c r="BZ23" s="24"/>
-      <c r="CA23" s="24"/>
-      <c r="CB23" s="24"/>
-      <c r="CC23" s="24"/>
-      <c r="CD23" s="24"/>
+      <c r="BW23" s="34"/>
+      <c r="BX23" s="35"/>
+      <c r="BY23" s="35"/>
+      <c r="BZ23" s="35"/>
+      <c r="CA23" s="35"/>
+      <c r="CB23" s="35"/>
+      <c r="CC23" s="35"/>
+      <c r="CD23" s="35"/>
       <c r="CE23" s="11"/>
       <c r="CF23" s="10"/>
       <c r="CG23" s="10"/>
@@ -3609,7 +3608,7 @@
       <c r="E24" s="22">
         <v>44730</v>
       </c>
-      <c r="F24" s="46">
+      <c r="F24" s="23">
         <v>0</v>
       </c>
       <c r="G24" s="10"/>
@@ -3680,14 +3679,14 @@
       <c r="BT24" s="11"/>
       <c r="BU24" s="11"/>
       <c r="BV24" s="11"/>
-      <c r="BW24" s="31"/>
-      <c r="BX24" s="31"/>
-      <c r="BY24" s="31"/>
-      <c r="BZ24" s="31"/>
-      <c r="CA24" s="31"/>
-      <c r="CB24" s="31"/>
-      <c r="CC24" s="31"/>
-      <c r="CD24" s="31"/>
+      <c r="BW24" s="42"/>
+      <c r="BX24" s="42"/>
+      <c r="BY24" s="42"/>
+      <c r="BZ24" s="42"/>
+      <c r="CA24" s="42"/>
+      <c r="CB24" s="42"/>
+      <c r="CC24" s="42"/>
+      <c r="CD24" s="42"/>
       <c r="CE24" s="11"/>
       <c r="CF24" s="10"/>
       <c r="CG24" s="10"/>
@@ -4459,19 +4458,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:U2"/>
-    <mergeCell ref="V2:AZ2"/>
-    <mergeCell ref="BI22:BQ22"/>
-    <mergeCell ref="AD14:AQ14"/>
-    <mergeCell ref="AD15:AQ15"/>
-    <mergeCell ref="AR16:BC16"/>
-    <mergeCell ref="AR17:BC17"/>
-    <mergeCell ref="AD13:BV13"/>
-    <mergeCell ref="AX18:BV18"/>
-    <mergeCell ref="BD19:BL19"/>
-    <mergeCell ref="BD20:BL20"/>
-    <mergeCell ref="BI21:BQ21"/>
     <mergeCell ref="BW23:CD23"/>
     <mergeCell ref="BA2:CD2"/>
     <mergeCell ref="CE2:CQ2"/>
@@ -4488,6 +4474,19 @@
     <mergeCell ref="L7:R7"/>
     <mergeCell ref="P8:V8"/>
     <mergeCell ref="P9:V9"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:U2"/>
+    <mergeCell ref="V2:AZ2"/>
+    <mergeCell ref="BI22:BQ22"/>
+    <mergeCell ref="AD14:AQ14"/>
+    <mergeCell ref="AD15:AQ15"/>
+    <mergeCell ref="AR16:BC16"/>
+    <mergeCell ref="AR17:BC17"/>
+    <mergeCell ref="AD13:BV13"/>
+    <mergeCell ref="AX18:BV18"/>
+    <mergeCell ref="BD19:BL19"/>
+    <mergeCell ref="BD20:BL20"/>
+    <mergeCell ref="BI21:BQ21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F4:F24">

</xml_diff>